<commit_message>
ENH: change template and reformat code according to it
</commit_message>
<xml_diff>
--- a/regolith/templates/coa_template_nsf.xlsx
+++ b/regolith/templates/coa_template_nsf.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD1AD4-A631-9740-B649-CCEB757AD2E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NSF COA Template" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>G:</t>
   </si>
@@ -129,45 +130,6 @@
     </r>
   </si>
   <si>
-    <t>Alphaman, Alan K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test University XYZ </t>
-  </si>
-  <si>
-    <t>Test University ABC (adjunct)</t>
-  </si>
-  <si>
-    <t>Test University DEF (interviewed)</t>
-  </si>
-  <si>
-    <t>Department X</t>
-  </si>
-  <si>
-    <t>Alphaman2, Alice</t>
-  </si>
-  <si>
-    <t>Test University 1234</t>
-  </si>
-  <si>
-    <t>Alphaman3, Adam</t>
-  </si>
-  <si>
-    <t>example@example.com</t>
-  </si>
-  <si>
-    <t>Alphaman4, Ann</t>
-  </si>
-  <si>
-    <t>Journal ABC</t>
-  </si>
-  <si>
-    <t>Alphaman, Alexander</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
     <t>Last Active Date</t>
   </si>
   <si>
@@ -366,20 +328,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -409,27 +364,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -463,23 +398,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -491,7 +419,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -575,102 +503,55 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -681,47 +562,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -729,80 +570,59 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -810,7 +630,187 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1265,173 +1265,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1885,7 +1718,9 @@
       <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{43FFFF04-432E-7441-8B67-8EBB0629EF08}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1898,12 +1733,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TableA" displayName="TableA" ref="A16:D21" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TableA" displayName="TableA" ref="A16:D17" insertRow="1" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <tableColumns count="4">
-    <tableColumn id="1" name="1" dataDxfId="41"/>
-    <tableColumn id="2" name="Your Name:" dataDxfId="40"/>
-    <tableColumn id="3" name="Your Organizational Affiliation(s), last 12 mo" dataDxfId="39"/>
-    <tableColumn id="4" name="Last Active Date" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="1" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Your Name:" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Your Organizational Affiliation(s), last 12 mo" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Last Active Date" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1915,14 +1750,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableD23" displayName="TableD23" ref="A26:E31" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="A26:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TableD23" displayName="TableD23" ref="A22:E23" insertRow="1" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="A22:E23" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="2" dataDxfId="32"/>
-    <tableColumn id="2" name="Name:" dataDxfId="31"/>
-    <tableColumn id="3" name="Type of Relationship" dataDxfId="30"/>
-    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="29" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Last Active" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="2" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name:" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type of Relationship" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Optional  (email, Department)" dataDxfId="30" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Last Active" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1934,14 +1769,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="TableD" displayName="TableD" ref="A50:E55" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A50:E55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TableD" displayName="TableD" ref="A36:E38" totalsRowShown="0" headerRowDxfId="28" dataDxfId="5" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A36:E38" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="4" dataDxfId="23"/>
-    <tableColumn id="2" name="Name:" dataDxfId="22"/>
-    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="21"/>
-    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Last Active" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="4" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name:" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Organizational Affiliation" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Optional  (email, Department)" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Last Active" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1953,14 +1788,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TableD5" displayName="TableD5" ref="A61:E66" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A61:E66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TableD5" displayName="TableD5" ref="A44:E45" insertRow="1" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A44:E45" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="5" dataDxfId="13"/>
-    <tableColumn id="2" name="Name:" dataDxfId="12"/>
-    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="11"/>
-    <tableColumn id="4" name="Journal/Collection" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Last Active" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="5" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name:" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Organizational Affiliation" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Journal/Collection" dataDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Last Active" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1972,13 +1807,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="TableC" displayName="TableC" ref="A37:D44" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A37:D44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TableC" displayName="TableC" ref="A29:D30" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A29:D30" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="3" dataDxfId="3"/>
-    <tableColumn id="2" name="Advisor/Advisee Name:" dataDxfId="2"/>
-    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="1"/>
-    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="3" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Advisor/Advisee Name:" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Organizational Affiliation" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Optional  (email, Department)" dataDxfId="6" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2191,661 +2026,457 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R66"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="2.59765625" style="1" customWidth="1"/>
     <col min="7" max="17" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="2.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="2.3984375" style="1" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="20" max="16384" width="0" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="195.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-    </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-    </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" ht="67.349999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+    <row r="1" spans="1:5" ht="195.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" ht="62.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-    </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" ht="49.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" s="29" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+    </row>
+    <row r="38" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+    </row>
+    <row r="39" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+    </row>
+    <row r="40" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-    </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-    </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-    </row>
-    <row r="7" spans="1:5" s="10" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-    </row>
-    <row r="8" spans="1:5" ht="62.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-    </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-    </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-    </row>
-    <row r="15" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="45">
-        <v>42736</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="45">
-        <v>42716</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" s="12" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-    </row>
-    <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="7" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="14" t="s">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="C44" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
-    </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-    </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="37"/>
-    </row>
-    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="37"/>
-    </row>
-    <row r="32" spans="1:5" s="9" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D36" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="33"/>
-    </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="32"/>
-    </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="32"/>
-    </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="36"/>
-    </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="36"/>
-    </row>
-    <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="36"/>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="21">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="21"/>
-    </row>
-    <row r="53" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="21"/>
-    </row>
-    <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29"/>
-    </row>
-    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="30"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="31"/>
-    </row>
-    <row r="56" spans="1:5" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" s="38" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-    </row>
-    <row r="58" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E62" s="21">
-        <v>42736</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="21"/>
-    </row>
-    <row r="64" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="22"/>
-      <c r="B64" s="23"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="21"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="22"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="21"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="24"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="27"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="17"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="22">
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A57:E57"/>
+  <mergeCells count="23">
+    <mergeCell ref="A40:E40"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:E8"/>
@@ -2854,27 +2485,34 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A24:XFD24"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A51:A55">
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A37:A38" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"A:,C:"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"R:"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"G:,T:,P:"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62:A66">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A45" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"B:,E:"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A38:A44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"G:,T:"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1:E1" r:id="rId1" display="https://www.nsf.gov/bfa/dias/policy/coa.jsp"/>
+    <hyperlink ref="A1:E1" r:id="rId1" display="https://www.nsf.gov/bfa/dias/policy/coa.jsp" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" fitToHeight="0" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
DEV: delete the empty line in template
</commit_message>
<xml_diff>
--- a/regolith/templates/coa_template_nsf.xlsx
+++ b/regolith/templates/coa_template_nsf.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD1AD4-A631-9740-B649-CCEB757AD2E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB9BCB3-AC7B-D441-AB85-87734264DEEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,39 +590,39 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -633,186 +633,6 @@
   <dxfs count="45">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1265,6 +1085,167 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1277,6 +1258,25 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1769,14 +1769,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TableD" displayName="TableD" ref="A36:E38" totalsRowShown="0" headerRowDxfId="28" dataDxfId="5" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="A36:E38" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TableD" displayName="TableD" ref="A36:E37" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A36:E37" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="4" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name:" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Organizational Affiliation" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Optional  (email, Department)" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Last Active" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="4" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name:" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Organizational Affiliation" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Optional  (email, Department)" dataDxfId="20" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Last Active" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1788,14 +1788,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TableD5" displayName="TableD5" ref="A44:E45" insertRow="1" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A44:E45" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TableD5" displayName="TableD5" ref="A43:E44" insertRow="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A43:E44" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="5" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name:" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Organizational Affiliation" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Journal/Collection" dataDxfId="16" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Last Active" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="5" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name:" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Organizational Affiliation" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Journal/Collection" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Last Active" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1807,13 +1807,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TableC" displayName="TableC" ref="A29:D30" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TableC" displayName="TableC" ref="A29:D30" insertRow="1" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A29:D30" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="3" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Advisor/Advisee Name:" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Organizational Affiliation" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Optional  (email, Department)" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="3" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Advisor/Advisee Name:" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Organizational Affiliation" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Optional  (email, Department)" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2030,10 +2030,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2051,137 +2051,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="195.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:5" s="9" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" spans="1:5" ht="62.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" s="8" customFormat="1" ht="49.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
@@ -2209,13 +2209,13 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
@@ -2261,26 +2261,26 @@
       <c r="D23" s="16"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" s="29" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:5" s="36" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -2327,24 +2327,24 @@
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
@@ -2384,93 +2384,93 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-    </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-    </row>
-    <row r="39" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-    </row>
-    <row r="40" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="30" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+    </row>
+    <row r="39" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+    </row>
+    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
+      <c r="D42" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" s="3"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="17"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="23">
-    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A24:XFD24"/>
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A19:E19"/>
@@ -2486,16 +2486,9 @@
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A24:XFD24"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A37:A38" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A37" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"A:,C:"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A23" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -2504,7 +2497,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"G:,T:,P:"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A45" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A44" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"B:,E:"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30" xr:uid="{00000000-0002-0000-0000-000004000000}">

</xml_diff>

<commit_message>
DEV: fill in table3 BUG: debug the inst is None
</commit_message>
<xml_diff>
--- a/regolith/templates/coa_template_nsf.xlsx
+++ b/regolith/templates/coa_template_nsf.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB9BCB3-AC7B-D441-AB85-87734264DEEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3C940-2D09-9547-86CA-5BA052CE380C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,6 +408,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -508,50 +509,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -570,13 +531,9 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -595,35 +552,65 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -643,6 +630,54 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -762,29 +797,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -804,13 +816,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -826,7 +831,8 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -835,12 +841,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1002,29 +1002,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1044,13 +1021,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1066,7 +1036,8 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1075,12 +1046,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1097,7 +1062,7 @@
       </font>
       <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1108,8 +1073,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1130,7 +1093,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1141,8 +1104,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1163,7 +1124,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1174,8 +1135,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1196,7 +1155,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1207,8 +1166,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1229,7 +1186,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1240,24 +1197,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1279,13 +1220,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1301,6 +1235,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1471,6 +1406,171 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1494,25 +1594,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1520,21 +1601,13 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1542,34 +1615,50 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1584,138 +1673,13 @@
           <color indexed="64"/>
         </bottom>
       </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -1733,12 +1697,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TableA" displayName="TableA" ref="A16:D17" insertRow="1" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TableA" displayName="TableA" ref="A16:D17" insertRow="1" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="1" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Your Name:" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Your Organizational Affiliation(s), last 12 mo" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Last Active Date" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="1" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Your Name:" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Your Organizational Affiliation(s), last 12 mo" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Last Active Date" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1750,14 +1714,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TableD23" displayName="TableD23" ref="A22:E23" insertRow="1" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TableD23" displayName="TableD23" ref="A22:E23" insertRow="1" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="A22:E23" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="2" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name:" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type of Relationship" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Optional  (email, Department)" dataDxfId="30" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Last Active" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="2" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name:" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type of Relationship" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Optional  (email, Department)" dataDxfId="23" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Last Active" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1769,14 +1733,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TableD" displayName="TableD" ref="A36:E37" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TableD" displayName="TableD" ref="A36:E37" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="A36:E37" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="4" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name:" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Organizational Affiliation" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Optional  (email, Department)" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Last Active" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="4" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name:" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Organizational Affiliation" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Optional  (email, Department)" dataDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Last Active" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1788,14 +1752,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TableD5" displayName="TableD5" ref="A43:E44" insertRow="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TableD5" displayName="TableD5" ref="A43:E44" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <autoFilter ref="A43:E44" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="5" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name:" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Organizational Affiliation" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Journal/Collection" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Last Active" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="5" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name:" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Organizational Affiliation" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Journal/Collection" dataDxfId="9" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Last Active" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1807,13 +1771,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TableC" displayName="TableC" ref="A29:D30" insertRow="1" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TableC" displayName="TableC" ref="A29:D30" insertRow="1" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A29:D30" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="3" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Advisor/Advisee Name:" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Organizational Affiliation" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Optional  (email, Department)" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="3" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Advisor/Advisee Name:" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Organizational Affiliation" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Optional  (email, Department)" dataDxfId="2" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2030,454 +1994,1091 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R694"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:E33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.3984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.59765625" style="1" customWidth="1"/>
-    <col min="7" max="17" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="2.3984375" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="16384" width="0" style="1" hidden="1"/>
+    <col min="1" max="1" width="4.3984375" style="27" customWidth="1"/>
+    <col min="2" max="2" width="22.3984375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="34.59765625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="29.3984375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="27" customWidth="1"/>
+    <col min="6" max="6" width="2.59765625" style="27" customWidth="1"/>
+    <col min="7" max="17" width="0" style="27" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="2.3984375" style="27" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0" style="27" hidden="1" customWidth="1"/>
+    <col min="20" max="16384" width="0" style="27" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="195.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:5" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" s="9" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:5" s="29" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" ht="62.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" ht="49.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="1:5" ht="49.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:5" s="18" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" s="18" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="7" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" s="36" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+    <row r="23" spans="1:5" s="18" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" s="18" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" s="18" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D28" s="7" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D28" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="18"/>
-    </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
+    <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" s="13" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="1:5" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="7" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="22"/>
+    </row>
+    <row r="35" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-    </row>
-    <row r="39" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
+    <row r="37" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-    </row>
-    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="22"/>
+    </row>
+    <row r="41" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="7" t="s">
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="17"/>
-    </row>
+    <row r="44" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="69" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="73" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="75" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="85" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="86" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="89" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="92" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="95" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="96" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="98" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="99" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="100" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="104" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="105" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="106" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="107" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="108" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="109" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="110" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="114" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="118" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="121" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="122" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="123" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="124" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="125" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="126" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="127" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="128" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="129" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="130" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="131" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="132" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="133" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="134" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="135" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="136" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="137" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="138" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="139" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="140" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="141" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="142" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="143" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="144" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="145" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="146" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="147" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="148" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="149" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="150" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="151" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="152" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="153" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="154" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="155" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="156" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="157" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="158" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="159" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="160" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="161" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="162" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="163" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="164" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="165" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="166" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="167" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="168" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="169" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="170" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="171" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="172" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="173" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="174" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="175" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="176" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="177" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="178" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="179" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="180" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="181" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="182" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="183" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="184" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="185" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="186" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="187" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="188" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="189" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="190" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="191" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="192" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="193" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="194" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="195" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="196" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="197" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="198" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="199" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="200" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="201" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="202" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="203" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="204" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="205" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="206" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="207" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="208" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="209" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="210" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="211" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="212" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="213" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="214" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="215" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="216" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="217" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="218" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="219" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="220" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="221" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="222" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="223" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="224" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="225" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="226" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="227" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="228" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="229" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="230" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="231" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="232" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="233" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="234" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="235" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="236" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="237" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="238" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="239" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="240" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="241" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="242" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="243" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="244" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="245" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="246" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="247" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="248" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="249" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="250" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="251" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="252" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="253" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="254" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="255" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="256" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="257" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="258" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="259" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="260" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="261" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="262" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="263" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="264" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="265" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="266" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="267" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="268" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="269" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="270" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="271" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="272" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="273" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="274" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="275" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="276" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="277" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="278" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="279" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="280" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="281" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="282" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="283" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="284" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="285" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="286" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="287" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="288" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="289" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="290" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="291" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="292" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="293" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="294" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="295" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="296" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="297" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="298" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="299" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="300" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="301" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="302" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="303" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="304" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="305" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="306" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="307" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="308" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="309" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="310" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="311" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="312" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="313" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="314" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="315" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="316" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="317" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="318" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="319" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="320" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="321" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="322" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="323" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="324" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="325" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="326" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="327" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="328" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="329" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="330" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="331" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="332" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="333" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="334" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="335" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="336" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="337" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="338" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="339" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="340" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="341" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="342" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="343" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="344" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="345" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="346" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="347" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="348" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="349" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="350" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="351" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="352" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="353" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="354" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="355" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="356" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="357" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="358" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="359" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="360" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="361" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="362" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="363" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="364" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="365" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="366" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="367" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="368" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="369" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="370" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="371" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="372" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="373" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="374" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="375" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="376" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="377" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="378" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="379" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="380" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="381" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="382" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="383" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="384" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="385" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="386" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="387" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="388" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="389" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="390" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="391" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="392" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="393" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="394" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="395" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="396" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="397" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="398" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="399" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="400" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="401" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="402" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="403" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="404" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="405" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="406" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="407" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="408" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="409" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="410" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="411" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="412" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="413" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="414" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="415" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="416" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="417" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="418" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="419" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="420" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="421" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="422" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="423" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="424" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="425" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="426" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="427" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="428" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="429" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="430" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="431" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="432" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="433" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="434" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="435" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="436" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="437" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="438" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="439" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="440" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="441" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="442" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="443" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="444" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="445" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="446" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="447" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="448" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="449" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="450" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="451" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="452" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="453" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="454" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="455" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="456" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="457" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="458" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="459" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="460" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="461" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="462" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="463" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="464" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="465" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="466" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="467" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="468" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="469" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="470" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="471" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="472" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="473" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="474" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="475" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="476" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="477" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="478" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="479" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="480" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="481" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="482" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="483" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="484" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="485" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="486" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="487" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="488" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="489" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="490" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="491" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="492" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="493" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="494" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="495" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="496" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="497" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="498" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="499" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="500" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="501" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="502" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="503" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="504" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="505" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="506" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="507" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="508" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="509" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="510" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="511" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="512" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="513" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="514" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="515" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="516" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="517" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="518" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="519" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="520" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="521" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="522" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="523" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="524" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="525" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="526" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="527" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="528" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="529" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="530" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="531" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="532" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="533" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="534" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="535" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="536" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="537" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="538" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="539" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="540" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="541" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="542" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="543" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="544" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="545" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="546" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="547" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="548" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="549" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="550" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="551" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="552" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="553" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="554" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="555" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="556" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="557" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="558" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="559" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="560" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="561" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="562" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="563" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="564" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="565" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="566" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="567" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="568" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="569" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="570" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="571" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="572" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="573" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="574" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="575" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="576" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="577" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="578" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="579" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="580" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="581" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="582" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="583" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="584" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="585" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="586" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="587" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="588" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="589" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="590" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="591" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="592" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="593" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="594" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="595" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="596" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="597" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="598" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="599" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="600" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="601" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="602" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="603" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="604" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="605" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="606" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="607" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="608" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="609" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="610" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="611" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="612" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="613" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="614" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="615" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="616" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="617" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="618" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="619" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="620" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="621" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="622" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="623" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="624" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="625" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="626" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="627" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="628" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="629" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="630" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="631" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="632" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="633" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="634" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="635" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="636" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="637" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="638" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="639" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="640" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="641" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="642" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="643" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="644" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="645" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="646" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="647" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="648" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="649" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="650" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="651" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="652" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="653" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="654" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="655" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="656" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="657" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="658" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="659" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="660" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="661" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="662" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="663" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="664" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="665" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="666" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="667" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="668" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="669" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="670" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="671" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="672" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="673" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="674" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="675" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="676" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="677" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="678" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="679" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="680" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="681" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="682" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="683" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="684" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="685" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="686" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="687" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="688" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="689" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="690" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="691" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="692" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="693" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="694" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="23">
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A24:XFD24"/>
-    <mergeCell ref="A39:E39"/>
+  <mergeCells count="14">
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="A15:E15"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A11:E11"/>
@@ -2485,7 +3086,11 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A37" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>